<commit_message>
Modified as per new Assessment Creation flow
</commit_message>
<xml_diff>
--- a/src/main/resources/com/kh/IRA/TestData/TestData.xlsx
+++ b/src/main/resources/com/kh/IRA/TestData/TestData.xlsx
@@ -12,12 +12,12 @@
     <sheet name="CreateAssessment" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <oleSize ref="D2:M6"/>
+  <oleSize ref="A6:J10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>TC No</t>
   </si>
@@ -153,7 +153,7 @@
     <t>90</t>
   </si>
   <si>
-    <t>24/03/20 13:00</t>
+    <t>30/03/20 17:20</t>
   </si>
   <si>
     <t>31/03/20 23:59</t>
@@ -200,17 +200,41 @@
   <si>
     <t>60</t>
   </si>
+  <si>
+    <t>CreateFree</t>
+  </si>
+  <si>
+    <t>Free_Assessment</t>
+  </si>
+  <si>
+    <t>Free_Assessment_Description</t>
+  </si>
+  <si>
+    <t>1.This online test requires a stable internet connection.
+2.We recommend using Chrome or Firefox browsers only.
+3.This test must be taken on the desktop only.
+4.The total time to complete the test is 60 mins(1 hr).
+5.This is a free assessment.
+7.If you run out of time, all attempted questions will be auto-submitted.
+8.For any technical queries, please email us at  support@knowledgehut.com.</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="dd\/mm\/yy\ hh:mm"/>
+    <numFmt numFmtId="176" formatCode="dd\/mm\/yy\ hh:mm"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -243,17 +267,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,6 +296,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -276,7 +313,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -290,9 +335,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -300,58 +369,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -365,9 +382,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -388,31 +412,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,7 +544,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,139 +580,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -579,17 +603,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -617,6 +630,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -632,16 +671,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -664,166 +703,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -835,7 +859,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -852,7 +876,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1314,13 +1338,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
   <cols>
     <col min="2" max="2" width="14.7142857142857" customWidth="1"/>
     <col min="3" max="3" width="18.8571428571429" customWidth="1"/>
@@ -1367,7 +1391,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" ht="180" spans="1:11">
+    <row r="2" ht="87" customHeight="1" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1402,7 +1426,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" ht="180" spans="1:11">
+    <row r="3" ht="125" customHeight="1" spans="1:11">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1505,6 +1529,41 @@
       </c>
       <c r="K5" s="11" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="6" ht="135" spans="1:11">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Date selection based on timezone
</commit_message>
<xml_diff>
--- a/src/main/resources/com/kh/IRA/TestData/TestData.xlsx
+++ b/src/main/resources/com/kh/IRA/TestData/TestData.xlsx
@@ -12,12 +12,12 @@
     <sheet name="CreateAssessment" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <oleSize ref="C3:L7"/>
+  <oleSize ref="C1:L5"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
   <si>
     <t>TC No</t>
   </si>
@@ -86,12 +86,6 @@
   </si>
   <si>
     <t>TimeZone</t>
-  </si>
-  <si>
-    <t>StartTime</t>
-  </si>
-  <si>
-    <t>EndTime</t>
   </si>
   <si>
     <t>Number of Questions</t>
@@ -125,9 +119,6 @@
     <t>Asia/Kolkata</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>CreateGroup</t>
   </si>
   <si>
@@ -150,13 +141,7 @@
     <t>70</t>
   </si>
   <si>
-    <t>90</t>
-  </si>
-  <si>
-    <t>27/04/20 20:00</t>
-  </si>
-  <si>
-    <t>31/03/21 23:59</t>
+    <t>60</t>
   </si>
   <si>
     <t>CreateRecall</t>
@@ -171,6 +156,9 @@
     <t>This is a recall quiz.
 No Pass percentage applicable
 No limits applicable</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>20</t>
@@ -226,12 +214,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="dd\/mm\/yy\ hh:mm"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -257,23 +244,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -288,56 +275,69 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -359,36 +359,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -415,181 +402,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -603,13 +590,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -638,6 +629,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -662,48 +677,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -727,128 +714,128 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -856,7 +843,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -873,7 +859,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1201,28 +1186,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="6.71428571428571" style="7" customWidth="1"/>
+    <col min="1" max="1" width="6.71428571428571" style="6" customWidth="1"/>
     <col min="2" max="2" width="14.4285714285714" customWidth="1"/>
     <col min="3" max="3" width="33.2857142857143" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" spans="1:4">
-      <c r="A1" s="8" t="s">
+    <row r="1" s="5" customFormat="1" spans="1:4">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="7">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1236,13 +1221,13 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="7">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
@@ -1250,7 +1235,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1264,7 +1249,7 @@
       </c>
     </row>
     <row r="8" spans="5:5">
-      <c r="E8" s="10"/>
+      <c r="E8" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1290,24 +1275,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1324,7 +1309,7 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="5"/>
+      <c r="A3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1335,10 +1320,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
@@ -1349,11 +1334,10 @@
     <col min="5" max="5" width="60.8571428571429" customWidth="1"/>
     <col min="6" max="6" width="16.1428571428571" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="10" width="16.7142857142857" customWidth="1"/>
-    <col min="11" max="11" width="11.8571428571429" customWidth="1"/>
+    <col min="9" max="9" width="11.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="30" spans="1:11">
+    <row r="1" s="1" customFormat="1" ht="30" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1381,186 +1365,150 @@
       <c r="I1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="2" ht="87" customHeight="1" spans="1:11">
+    <row r="2" ht="87" customHeight="1" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="H2" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>31</v>
+      <c r="I2" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="3" ht="125" customHeight="1" spans="1:11">
+    <row r="3" ht="125" customHeight="1" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>39</v>
-      </c>
       <c r="H3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>39</v>
+        <v>30</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="4" ht="45" spans="1:11">
+    <row r="4" ht="45" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>46</v>
-      </c>
     </row>
-    <row r="5" ht="105" spans="1:11">
+    <row r="5" ht="105" spans="1:9">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>52</v>
-      </c>
     </row>
-    <row r="6" ht="135" spans="1:11">
+    <row r="6" ht="135" spans="1:9">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C6" t="s">
+      <c r="G6" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>46</v>
+      <c r="H6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IRA changed to PRISM
</commit_message>
<xml_diff>
--- a/src/main/resources/com/kh/IRA/TestData/TestData.xlsx
+++ b/src/main/resources/com/kh/IRA/TestData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdityaPrasad\Desktop\SeleniumScript\IRA\src\main\resources\com\kh\IRA\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2ABC5754-21FB-4381-A7A7-FAD6A5BBCB8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208C0551-BDE8-4590-A4FF-2AA6F63D6EF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCredentials" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="56">
   <si>
     <t>TC No</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>CALogin</t>
-  </si>
-  <si>
-    <t>authorprod@mailinator.com</t>
   </si>
   <si>
     <t>ManagerLogin</t>
@@ -213,6 +210,12 @@
 6.The test comprises of 4 questions. There will be no negative marks for wrong answers.
 7.If you run out of time, all attempted questions will be auto-submitted.
 8.For any technical queries, please email us at  aditya.prasad@knowledgehut.co.</t>
+  </si>
+  <si>
+    <t>authorprod@knowledgehut.com</t>
+  </si>
+  <si>
+    <t>Password@123</t>
   </si>
 </sst>
 </file>
@@ -298,13 +301,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -591,7 +594,7 @@
     <col min="1" max="1" width="6.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="33.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
@@ -630,11 +633,11 @@
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>3</v>
+      <c r="C3" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -642,17 +645,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="E8" s="11"/>
+      <c r="E8" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -664,7 +667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -685,34 +688,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="12">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="12"/>
+      <c r="A3" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -747,25 +750,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="87" customHeight="1">
@@ -773,28 +776,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="I2" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="125.1" customHeight="1">
@@ -802,28 +805,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="H3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="45">
@@ -831,28 +834,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="105">
@@ -860,28 +863,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="135">
@@ -889,28 +892,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="H6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed LMS end Login And Logout
</commit_message>
<xml_diff>
--- a/src/main/resources/com/kh/IRA/TestData/TestData.xlsx
+++ b/src/main/resources/com/kh/IRA/TestData/TestData.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6FB06F7A-FC7E-445E-A387-A1F5CF96E5C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdityaPrasad\Desktop\SeleniumScript\IRA\src\main\resources\com\kh\IRA\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C156212-0B75-4223-AEEF-A5FB1F1F163E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="20760" windowHeight="11820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCredentials" sheetId="1" r:id="rId1"/>
@@ -13,12 +18,11 @@
     <sheet name="CreateAssessment" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A4:E6"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
   <si>
     <t>TC No</t>
   </si>
@@ -35,16 +39,10 @@
     <t>LearnerLogin</t>
   </si>
   <si>
-    <t>learnerprod@mailinator.com</t>
-  </si>
-  <si>
     <t>CALogin</t>
   </si>
   <si>
     <t>ManagerLogin</t>
-  </si>
-  <si>
-    <t>managerprod@mailinator.com</t>
   </si>
   <si>
     <t>Skill</t>
@@ -208,17 +206,20 @@
 8.For any technical queries, please email us at  aditya.prasad@knowledgehut.co.</t>
   </si>
   <si>
-    <t>authorprod@knowledgehut.com</t>
-  </si>
-  <si>
     <t>Password@123</t>
+  </si>
+  <si>
+    <t>y.adityaprasad@gmail.com</t>
+  </si>
+  <si>
+    <t>khmanagertest@khcodelab.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +231,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -273,10 +282,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -304,8 +314,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -581,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -615,11 +627,11 @@
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
+      <c r="C2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -627,35 +639,35 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>55</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="9">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="E8" s="10"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{66E763F9-885C-48F7-A817-E00ACB40867D}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{740EF9BA-B123-476E-9EBA-EF05E814D40E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -684,13 +696,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -698,16 +710,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -723,7 +735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+    <sheetView topLeftCell="E4" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -746,25 +758,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="87" customHeight="1">
@@ -772,28 +784,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="I2" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="125.1" customHeight="1">
@@ -801,28 +813,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="G3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="H3" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="45">
@@ -830,28 +842,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="G4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="105">
@@ -859,28 +871,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="E5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="G5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="135">
@@ -888,28 +900,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="E6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="G6" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="H6" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>